<commit_message>
misc changes to expenses
added invoice and formatted spreadsheet
</commit_message>
<xml_diff>
--- a/Invoices/expenses_Paid.xlsx
+++ b/Invoices/expenses_Paid.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19935" windowHeight="12555" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Carlos Mariscal</t>
   </si>
@@ -46,13 +46,29 @@
   </si>
   <si>
     <t>goodwill (12V bricks)</t>
+  </si>
+  <si>
+    <t>Saida Ahker</t>
+  </si>
+  <si>
+    <t>LockBox boards</t>
+  </si>
+  <si>
+    <t>LCD Board</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>digikey LCD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
@@ -72,7 +88,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -80,19 +96,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -418,55 +452,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A2:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.875" customWidth="1"/>
+    <col min="2" max="2" width="15.625" customWidth="1"/>
+    <col min="3" max="3" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26">
-      <c r="A2" t="s">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1">
-        <v>33.83</v>
-      </c>
-      <c r="E2" s="1">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1">
-        <v>21</v>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -489,15 +504,19 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -519,15 +538,17 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="B4" s="3">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -549,15 +570,19 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>33.83</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
+        <v>17.13</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -579,8 +604,157 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3">
+        <v>26.6</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3">
+        <v>24</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5">
+        <f>SUM(B3:B14)</f>
+        <v>79.83</v>
+      </c>
+      <c r="C15" s="5">
+        <f t="shared" ref="C15:F15" si="0">SUM(C3:C14)</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" si="0"/>
+        <v>106.03</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added my expenses to the expenses_Paid.xlsx
</commit_message>
<xml_diff>
--- a/Invoices/expenses_Paid.xlsx
+++ b/Invoices/expenses_Paid.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19940" windowHeight="12560" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Carlos Mariscal</t>
   </si>
@@ -68,8 +68,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -111,11 +111,11 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,7 +455,7 @@
   <dimension ref="A2:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -666,8 +666,13 @@
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:26">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3">
+        <v>31.37</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -703,7 +708,7 @@
       </c>
       <c r="C15" s="5">
         <f t="shared" ref="C15:F15" si="0">SUM(C3:C14)</f>
-        <v>0</v>
+        <v>31.37</v>
       </c>
       <c r="D15" s="5">
         <f t="shared" si="0"/>
@@ -755,7 +760,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>